<commit_message>
Updated elevation column to elevation_change
Util para saber, após ter pesquisado para não confundir com possível altitude da pista
</commit_message>
<xml_diff>
--- a/n2k_data.xlsx
+++ b/n2k_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Facudadi\Year 3 - Winter\Capstone Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D12B5E6-3343-40B6-8106-BAE3BDC4FDB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B9F82C-0419-4BED-83AA-5409A9B6FEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B5482C47-ED50-4964-B6D7-8B982CE462CC}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B5482C47-ED50-4964-B6D7-8B982CE462CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -170,10 +170,10 @@
     <t>turns</t>
   </si>
   <si>
-    <t>elevation</t>
-  </si>
-  <si>
     <t>top_speed</t>
+  </si>
+  <si>
+    <t>elevation_change</t>
   </si>
 </sst>
 </file>
@@ -209,10 +209,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,7 +528,7 @@
   <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,8 +538,8 @@
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="10.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="10.42578125" customWidth="1"/>
     <col min="21" max="21" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="23.7109375" bestFit="1" customWidth="1"/>
@@ -600,14 +598,14 @@
       <c r="Q1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" t="s">
         <v>43</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" t="s">
         <v>44</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="U1" t="s">
         <v>39</v>
@@ -674,25 +672,25 @@
       <c r="Q2">
         <v>5.4119999999999999</v>
       </c>
-      <c r="R2" s="1">
+      <c r="R2">
         <v>15</v>
       </c>
-      <c r="S2" s="1">
+      <c r="S2">
         <v>16.8</v>
       </c>
-      <c r="T2" s="1">
+      <c r="T2">
         <v>327.9</v>
       </c>
-      <c r="U2" s="1">
+      <c r="U2">
         <v>-3.5</v>
       </c>
-      <c r="V2" s="1">
+      <c r="V2">
         <v>-2</v>
       </c>
-      <c r="W2" s="1">
+      <c r="W2">
         <v>21</v>
       </c>
-      <c r="X2" s="1">
+      <c r="X2">
         <v>18.5</v>
       </c>
     </row>
@@ -748,25 +746,25 @@
       <c r="Q3">
         <v>6.1740000000000004</v>
       </c>
-      <c r="R3" s="1">
+      <c r="R3">
         <v>27</v>
       </c>
-      <c r="S3" s="1">
+      <c r="S3">
         <v>2.48</v>
       </c>
-      <c r="T3" s="1">
+      <c r="T3">
         <v>334.6</v>
       </c>
-      <c r="U3" s="1">
+      <c r="U3">
         <v>-3.25</v>
       </c>
-      <c r="V3" s="1">
+      <c r="V3">
         <v>-1.75</v>
       </c>
-      <c r="W3" s="1">
+      <c r="W3">
         <v>22.5</v>
       </c>
-      <c r="X3" s="1">
+      <c r="X3">
         <v>21</v>
       </c>
     </row>
@@ -822,25 +820,25 @@
       <c r="Q4">
         <v>5.2779999999999996</v>
       </c>
-      <c r="R4" s="1">
+      <c r="R4">
         <v>14</v>
       </c>
-      <c r="S4" s="1">
+      <c r="S4">
         <v>2.44</v>
       </c>
-      <c r="T4" s="1">
+      <c r="T4">
         <v>326.2</v>
       </c>
-      <c r="U4" s="1">
+      <c r="U4">
         <v>-3.25</v>
       </c>
-      <c r="V4" s="1">
+      <c r="V4">
         <v>-1.75</v>
       </c>
-      <c r="W4" s="1">
+      <c r="W4">
         <v>23</v>
       </c>
-      <c r="X4" s="1">
+      <c r="X4">
         <v>21</v>
       </c>
     </row>
@@ -873,13 +871,13 @@
       <c r="Q5">
         <v>6.0030000000000001</v>
       </c>
-      <c r="R5" s="1">
+      <c r="R5">
         <v>20</v>
       </c>
-      <c r="S5" s="1">
+      <c r="S5">
         <v>26.96</v>
       </c>
-      <c r="T5" s="1">
+      <c r="T5">
         <v>351.8</v>
       </c>
     </row>
@@ -912,18 +910,18 @@
       <c r="Q6">
         <v>5.4119999999999999</v>
       </c>
-      <c r="R6" s="1">
+      <c r="R6">
         <v>19</v>
       </c>
-      <c r="S6" s="1">
+      <c r="S6">
         <v>3.53</v>
       </c>
-      <c r="T6" s="1">
+      <c r="T6">
         <v>349.3</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>22</v>
       </c>
       <c r="B7">
@@ -974,13 +972,13 @@
       <c r="Q7">
         <v>3.3370000000000002</v>
       </c>
-      <c r="R7" s="1">
+      <c r="R7">
         <v>19</v>
       </c>
-      <c r="S7" s="1">
+      <c r="S7">
         <v>41.95</v>
       </c>
-      <c r="T7" s="1">
+      <c r="T7">
         <v>289</v>
       </c>
       <c r="U7">
@@ -997,7 +995,7 @@
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>24</v>
       </c>
       <c r="B8">
@@ -1048,13 +1046,13 @@
       <c r="Q8">
         <v>4.657</v>
       </c>
-      <c r="R8" s="1">
+      <c r="R8">
         <v>14</v>
       </c>
-      <c r="S8" s="1">
+      <c r="S8">
         <v>29.63</v>
       </c>
-      <c r="T8" s="1">
+      <c r="T8">
         <v>307.2</v>
       </c>
       <c r="U8">
@@ -1071,7 +1069,7 @@
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>25</v>
       </c>
       <c r="B9">
@@ -1122,13 +1120,13 @@
       <c r="Q9">
         <v>4.3609999999999998</v>
       </c>
-      <c r="R9" s="1">
+      <c r="R9">
         <v>14</v>
       </c>
-      <c r="S9" s="1">
+      <c r="S9">
         <v>5.25</v>
       </c>
-      <c r="T9" s="1">
+      <c r="T9">
         <v>342.7</v>
       </c>
       <c r="U9">
@@ -1145,7 +1143,7 @@
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>26</v>
       </c>
       <c r="B10">
@@ -1196,13 +1194,13 @@
       <c r="Q10">
         <v>4.3179999999999996</v>
       </c>
-      <c r="R10" s="1">
+      <c r="R10">
         <v>10</v>
       </c>
-      <c r="S10" s="1">
+      <c r="S10">
         <v>63.4</v>
       </c>
-      <c r="T10" s="1">
+      <c r="T10">
         <v>324.7</v>
       </c>
       <c r="U10">
@@ -1219,7 +1217,7 @@
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>27</v>
       </c>
       <c r="B11">
@@ -1270,13 +1268,13 @@
       <c r="Q11">
         <v>5.891</v>
       </c>
-      <c r="R11" s="1">
+      <c r="R11">
         <v>18</v>
       </c>
-      <c r="S11" s="1">
+      <c r="S11">
         <v>11.31</v>
       </c>
-      <c r="T11" s="1">
+      <c r="T11">
         <v>332.6</v>
       </c>
       <c r="U11">
@@ -1293,7 +1291,7 @@
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>23</v>
       </c>
       <c r="B12">
@@ -1344,13 +1342,13 @@
       <c r="Q12">
         <v>4.3810000000000002</v>
       </c>
-      <c r="R12" s="1">
+      <c r="R12">
         <v>14</v>
       </c>
-      <c r="S12" s="1">
+      <c r="S12">
         <v>34.619999999999997</v>
       </c>
-      <c r="T12" s="1">
+      <c r="T12">
         <v>310.3</v>
       </c>
       <c r="U12">
@@ -1367,7 +1365,7 @@
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>28</v>
       </c>
       <c r="B13">
@@ -1418,13 +1416,13 @@
       <c r="Q13">
         <v>7.0039999999999996</v>
       </c>
-      <c r="R13" s="1">
+      <c r="R13">
         <v>19</v>
       </c>
-      <c r="S13" s="1">
+      <c r="S13">
         <v>1012.1</v>
       </c>
-      <c r="T13" s="1">
+      <c r="T13">
         <v>350.8</v>
       </c>
       <c r="U13">
@@ -1441,7 +1439,7 @@
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>29</v>
       </c>
       <c r="B14">
@@ -1492,13 +1490,13 @@
       <c r="Q14">
         <v>4.2590000000000003</v>
       </c>
-      <c r="R14" s="1">
+      <c r="R14">
         <v>14</v>
       </c>
-      <c r="S14" s="1">
+      <c r="S14">
         <v>8.65</v>
       </c>
-      <c r="T14" s="1">
+      <c r="T14">
         <v>327.5</v>
       </c>
       <c r="U14">
@@ -1515,7 +1513,7 @@
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" t="s">
         <v>30</v>
       </c>
       <c r="B15">
@@ -1566,13 +1564,13 @@
       <c r="Q15">
         <v>5.7930000000000001</v>
       </c>
-      <c r="R15" s="1">
+      <c r="R15">
         <v>11</v>
       </c>
-      <c r="S15" s="1">
+      <c r="S15">
         <v>12.48</v>
       </c>
-      <c r="T15" s="1">
+      <c r="T15">
         <v>356.4</v>
       </c>
       <c r="U15">
@@ -1589,7 +1587,7 @@
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" t="s">
         <v>31</v>
       </c>
       <c r="B16">
@@ -1640,13 +1638,13 @@
       <c r="Q16">
         <v>4.9400000000000004</v>
       </c>
-      <c r="R16" s="1">
+      <c r="R16">
         <v>19</v>
       </c>
-      <c r="S16" s="1">
+      <c r="S16">
         <v>5.3</v>
       </c>
-      <c r="T16" s="1">
+      <c r="T16">
         <v>317.3</v>
       </c>
       <c r="U16">
@@ -1663,7 +1661,7 @@
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>32</v>
       </c>
       <c r="B17">
@@ -1714,13 +1712,13 @@
       <c r="Q17">
         <v>5.8070000000000004</v>
       </c>
-      <c r="R17" s="1">
+      <c r="R17">
         <v>18</v>
       </c>
-      <c r="S17" s="1">
+      <c r="S17">
         <v>40.43</v>
       </c>
-      <c r="T17" s="1">
+      <c r="T17">
         <v>305.7</v>
       </c>
       <c r="U17">
@@ -1737,7 +1735,7 @@
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>33</v>
       </c>
       <c r="B18">
@@ -1788,13 +1786,13 @@
       <c r="Q18">
         <v>5.4189999999999996</v>
       </c>
-      <c r="R18" s="1">
+      <c r="R18">
         <v>16</v>
       </c>
-      <c r="S18" s="1">
+      <c r="S18">
         <v>4.1779999999999999</v>
       </c>
-      <c r="T18" s="1">
+      <c r="T18">
         <v>322</v>
       </c>
       <c r="U18">
@@ -1811,7 +1809,7 @@
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>34</v>
       </c>
       <c r="B19">
@@ -1862,13 +1860,13 @@
       <c r="Q19">
         <v>5.5129999999999999</v>
       </c>
-      <c r="R19" s="1">
+      <c r="R19">
         <v>20</v>
       </c>
-      <c r="S19" s="1">
+      <c r="S19">
         <v>30.9</v>
       </c>
-      <c r="T19" s="1">
+      <c r="T19">
         <v>344.7</v>
       </c>
       <c r="U19">
@@ -1885,7 +1883,7 @@
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>35</v>
       </c>
       <c r="B20">
@@ -1936,13 +1934,13 @@
       <c r="Q20">
         <v>4.3040000000000003</v>
       </c>
-      <c r="R20" s="1">
+      <c r="R20">
         <v>17</v>
       </c>
-      <c r="S20" s="1">
+      <c r="S20">
         <v>2.6749999999999998</v>
       </c>
-      <c r="T20" s="1">
+      <c r="T20">
         <v>356.9</v>
       </c>
       <c r="U20">
@@ -1959,7 +1957,7 @@
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>36</v>
       </c>
       <c r="B21">
@@ -2010,13 +2008,13 @@
       <c r="Q21">
         <v>4.3090000000000002</v>
       </c>
-      <c r="R21" s="1">
+      <c r="R21">
         <v>15</v>
       </c>
-      <c r="S21" s="1">
+      <c r="S21">
         <v>42.98</v>
       </c>
-      <c r="T21" s="1">
+      <c r="T21">
         <v>338.3</v>
       </c>
       <c r="U21">
@@ -2033,7 +2031,7 @@
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>37</v>
       </c>
       <c r="B22">
@@ -2084,10 +2082,10 @@
       <c r="Q22">
         <v>6.2009999999999996</v>
       </c>
-      <c r="R22" s="1">
+      <c r="R22">
         <v>17</v>
       </c>
-      <c r="T22" s="1">
+      <c r="T22">
         <v>342</v>
       </c>
       <c r="U22">
@@ -2104,7 +2102,7 @@
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" t="s">
         <v>38</v>
       </c>
       <c r="B23">
@@ -2155,13 +2153,13 @@
       <c r="Q23">
         <v>5.2809999999999997</v>
       </c>
-      <c r="R23" s="1">
+      <c r="R23">
         <v>16</v>
       </c>
-      <c r="S23" s="1">
+      <c r="S23">
         <v>10.23</v>
       </c>
-      <c r="T23" s="1">
+      <c r="T23">
         <v>334.3</v>
       </c>
       <c r="U23">

</xml_diff>